<commit_message>
Finish new subgroup quantiles computation with the filtered data.
</commit_message>
<xml_diff>
--- a/data/studies-with-filtering-info.xlsx
+++ b/data/studies-with-filtering-info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="15600" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="15600" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="vals" sheetId="6" r:id="rId1"/>
@@ -6591,8 +6591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6612,7 +6612,7 @@
         <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
         <v>43</v>
@@ -13731,7 +13731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update data with Douwe's selection
 - includes changing myalgia event rate in WOSCOPS
</commit_message>
<xml_diff>
--- a/data/studies-with-filtering-info.xlsx
+++ b/data/studies-with-filtering-info.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="642" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="321" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="vals" sheetId="1" state="visible" r:id="rId2"/>
@@ -97,9 +97,6 @@
     <t>Primary Prevention</t>
   </si>
   <si>
-    <t>y</t>
-  </si>
-  <si>
     <t>ACAPS</t>
   </si>
   <si>
@@ -107,6 +104,9 @@
   </si>
   <si>
     <t>KAPS</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
   <si>
     <t>WOSCOPS</t>
@@ -218,12 +218,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -260,7 +266,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -269,7 +275,19 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -293,7 +311,7 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -345,8 +363,8 @@
   </sheetPr>
   <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C62" activeCellId="0" sqref="C62"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -403,7 +421,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -445,7 +463,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>22</v>
       </c>
@@ -487,7 +505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>22</v>
       </c>
@@ -529,7 +547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>22</v>
       </c>
@@ -571,7 +589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>22</v>
       </c>
@@ -613,7 +631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>22</v>
       </c>
@@ -655,7 +673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -697,7 +715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>4</v>
       </c>
@@ -739,7 +757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>22</v>
       </c>
@@ -781,7 +799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>4</v>
       </c>
@@ -823,7 +841,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>22</v>
       </c>
@@ -865,7 +883,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>22</v>
       </c>
@@ -907,7 +925,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>23</v>
       </c>
@@ -949,7 +967,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>22</v>
       </c>
@@ -991,7 +1009,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>24</v>
       </c>
@@ -1000,10 +1018,10 @@
         <v>p</v>
       </c>
       <c r="C16" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="E16" s="1" t="n">
         <v>0</v>
@@ -1036,7 +1054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>22</v>
       </c>
@@ -1078,7 +1096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>4</v>
       </c>
@@ -1120,7 +1138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>24</v>
       </c>
@@ -1129,10 +1147,10 @@
         <v>p</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E19" s="1" t="n">
         <v>3</v>
@@ -1165,7 +1183,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>22</v>
       </c>
@@ -1207,7 +1225,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>22</v>
       </c>
@@ -1249,7 +1267,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>22</v>
       </c>
@@ -1291,7 +1309,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>22</v>
       </c>
@@ -1333,7 +1351,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>24</v>
       </c>
@@ -1342,10 +1360,10 @@
         <v>p</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E24" s="1" t="n">
         <v>2</v>
@@ -1378,7 +1396,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>22</v>
       </c>
@@ -1420,52 +1438,52 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="26" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="0" t="str">
+      <c r="B26" s="2" t="str">
         <f aca="false">VLOOKUP(LEFT(A26, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="1" t="n">
+      <c r="E26" s="3" t="n">
         <v>46</v>
       </c>
-      <c r="F26" s="1" t="n">
+      <c r="F26" s="3" t="n">
         <v>3302</v>
       </c>
-      <c r="G26" s="1" t="n">
+      <c r="G26" s="3" t="n">
         <v>51</v>
       </c>
-      <c r="H26" s="1" t="n">
+      <c r="H26" s="3" t="n">
         <v>3293</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K26" s="1" t="n">
+      <c r="I26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="L26" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N26" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L26" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N26" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>22</v>
       </c>
@@ -1507,7 +1525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>22</v>
       </c>
@@ -1549,7 +1567,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>22</v>
       </c>
@@ -1591,7 +1609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>22</v>
       </c>
@@ -1633,52 +1651,52 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+    <row r="31" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="0" t="str">
+      <c r="B31" s="2" t="str">
         <f aca="false">VLOOKUP(LEFT(A31, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="1" t="n">
+      <c r="E31" s="3" t="n">
         <v>209</v>
       </c>
-      <c r="F31" s="1" t="n">
+      <c r="F31" s="3" t="n">
         <v>5170</v>
       </c>
-      <c r="G31" s="1" t="n">
+      <c r="G31" s="3" t="n">
         <v>231</v>
       </c>
-      <c r="H31" s="1" t="n">
+      <c r="H31" s="3" t="n">
         <v>5185</v>
       </c>
-      <c r="I31" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K31" s="1" t="n">
+      <c r="I31" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="L31" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N31" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L31" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N31" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>4</v>
       </c>
@@ -1720,7 +1738,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>22</v>
       </c>
@@ -1762,7 +1780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>22</v>
       </c>
@@ -1804,7 +1822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>22</v>
       </c>
@@ -1846,7 +1864,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>22</v>
       </c>
@@ -1888,7 +1906,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>22</v>
       </c>
@@ -1930,7 +1948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>24</v>
       </c>
@@ -1975,7 +1993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>4</v>
       </c>
@@ -2017,7 +2035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>22</v>
       </c>
@@ -2059,7 +2077,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>22</v>
       </c>
@@ -2101,7 +2119,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>22</v>
       </c>
@@ -2143,7 +2161,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>22</v>
       </c>
@@ -2185,7 +2203,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>22</v>
       </c>
@@ -2227,7 +2245,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>22</v>
       </c>
@@ -2269,7 +2287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>4</v>
       </c>
@@ -2311,7 +2329,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>4</v>
       </c>
@@ -2353,7 +2371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>22</v>
       </c>
@@ -2395,7 +2413,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>22</v>
       </c>
@@ -2437,7 +2455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>22</v>
       </c>
@@ -2479,7 +2497,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>24</v>
       </c>
@@ -2488,7 +2506,7 @@
         <v>p</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>32</v>
@@ -2524,7 +2542,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>22</v>
       </c>
@@ -2566,7 +2584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>22</v>
       </c>
@@ -2608,7 +2626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>24</v>
       </c>
@@ -2617,7 +2635,7 @@
         <v>p</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>33</v>
@@ -2653,7 +2671,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>22</v>
       </c>
@@ -2695,7 +2713,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>22</v>
       </c>
@@ -2737,7 +2755,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>24</v>
       </c>
@@ -2782,7 +2800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>22</v>
       </c>
@@ -2824,7 +2842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>24</v>
       </c>
@@ -2869,7 +2887,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>22</v>
       </c>
@@ -2911,52 +2929,52 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+    <row r="61" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B61" s="0" t="str">
+      <c r="B61" s="2" t="str">
         <f aca="false">VLOOKUP(LEFT(A61, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D61" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E61" s="1" t="n">
+      <c r="E61" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="F61" s="1" t="n">
+      <c r="F61" s="3" t="n">
         <v>3304</v>
       </c>
-      <c r="G61" s="1" t="n">
+      <c r="G61" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="H61" s="1" t="n">
+      <c r="H61" s="3" t="n">
         <v>3301</v>
       </c>
-      <c r="I61" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J61" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K61" s="1" t="n">
+      <c r="I61" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K61" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="L61" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="M61" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N61" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L61" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M61" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N61" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>4</v>
       </c>
@@ -3017,8 +3035,8 @@
   </sheetPr>
   <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C63" activeCellId="0" sqref="C63"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3083,7 +3101,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -3134,7 +3152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>22</v>
       </c>
@@ -3185,7 +3203,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>4</v>
       </c>
@@ -3236,7 +3254,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>22</v>
       </c>
@@ -3287,7 +3305,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>22</v>
       </c>
@@ -3338,7 +3356,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>22</v>
       </c>
@@ -3389,7 +3407,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -3440,7 +3458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>23</v>
       </c>
@@ -3491,7 +3509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>22</v>
       </c>
@@ -3542,7 +3560,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>22</v>
       </c>
@@ -3593,7 +3611,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>4</v>
       </c>
@@ -3644,7 +3662,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>22</v>
       </c>
@@ -3695,7 +3713,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>4</v>
       </c>
@@ -3746,7 +3764,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>4</v>
       </c>
@@ -3797,7 +3815,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>22</v>
       </c>
@@ -3848,7 +3866,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>23</v>
       </c>
@@ -3899,7 +3917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>24</v>
       </c>
@@ -3908,7 +3926,7 @@
         <v>p</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>40</v>
@@ -3953,7 +3971,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>22</v>
       </c>
@@ -4004,61 +4022,61 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="0" t="str">
+      <c r="B20" s="2" t="str">
         <f aca="false">VLOOKUP(LEFT(A20, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="1" t="n">
+      <c r="E20" s="3" t="n">
         <v>116</v>
       </c>
-      <c r="F20" s="1" t="n">
+      <c r="F20" s="3" t="n">
         <v>3304</v>
       </c>
-      <c r="G20" s="1" t="n">
+      <c r="G20" s="3" t="n">
         <v>183</v>
       </c>
-      <c r="H20" s="1" t="n">
+      <c r="H20" s="3" t="n">
         <v>3301</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M20" s="1" t="n">
+      <c r="I20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M20" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="N20" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q20" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N20" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q20" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>24</v>
       </c>
@@ -4067,10 +4085,10 @@
         <v>p</v>
       </c>
       <c r="C21" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="E21" s="1" t="n">
         <v>5</v>
@@ -4112,7 +4130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>4</v>
       </c>
@@ -4163,7 +4181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>4</v>
       </c>
@@ -4214,7 +4232,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>22</v>
       </c>
@@ -4265,7 +4283,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>22</v>
       </c>
@@ -4316,7 +4334,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>22</v>
       </c>
@@ -4367,7 +4385,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>24</v>
       </c>
@@ -4376,7 +4394,7 @@
         <v>p</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>41</v>
@@ -4421,7 +4439,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>22</v>
       </c>
@@ -4472,7 +4490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>22</v>
       </c>
@@ -4523,7 +4541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>22</v>
       </c>
@@ -4574,7 +4592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>22</v>
       </c>
@@ -4625,7 +4643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>24</v>
       </c>
@@ -4634,10 +4652,10 @@
         <v>p</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E32" s="1" t="n">
         <v>5</v>
@@ -4679,7 +4697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>22</v>
       </c>
@@ -4730,61 +4748,61 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+    <row r="34" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="0" t="str">
+      <c r="B34" s="2" t="str">
         <f aca="false">VLOOKUP(LEFT(A34, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D34" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E34" s="1" t="n">
+      <c r="E34" s="3" t="n">
         <v>174</v>
       </c>
-      <c r="F34" s="1" t="n">
+      <c r="F34" s="3" t="n">
         <v>3302</v>
       </c>
-      <c r="G34" s="1" t="n">
+      <c r="G34" s="3" t="n">
         <v>248</v>
       </c>
-      <c r="H34" s="1" t="n">
+      <c r="H34" s="3" t="n">
         <v>3293</v>
       </c>
-      <c r="I34" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L34" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M34" s="1" t="n">
+      <c r="I34" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M34" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="N34" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="O34" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P34" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q34" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N34" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O34" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P34" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q34" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>22</v>
       </c>
@@ -4835,7 +4853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>22</v>
       </c>
@@ -4886,7 +4904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>22</v>
       </c>
@@ -4937,61 +4955,61 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+    <row r="38" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="0" t="str">
+      <c r="B38" s="2" t="str">
         <f aca="false">VLOOKUP(LEFT(A38, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D38" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E38" s="1" t="n">
+      <c r="E38" s="3" t="n">
         <v>380</v>
       </c>
-      <c r="F38" s="1" t="n">
+      <c r="F38" s="3" t="n">
         <v>5170</v>
       </c>
-      <c r="G38" s="1" t="n">
+      <c r="G38" s="3" t="n">
         <v>421</v>
       </c>
-      <c r="H38" s="1" t="n">
+      <c r="H38" s="3" t="n">
         <v>5185</v>
       </c>
-      <c r="I38" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M38" s="1" t="n">
+      <c r="I38" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M38" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="N38" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="O38" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P38" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q38" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N38" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O38" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P38" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q38" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>4</v>
       </c>
@@ -5042,7 +5060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>4</v>
       </c>
@@ -5093,7 +5111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>22</v>
       </c>
@@ -5144,7 +5162,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>4</v>
       </c>
@@ -5195,7 +5213,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>24</v>
       </c>
@@ -5249,7 +5267,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>22</v>
       </c>
@@ -5300,7 +5318,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>4</v>
       </c>
@@ -5351,7 +5369,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>4</v>
       </c>
@@ -5402,7 +5420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>4</v>
       </c>
@@ -5453,7 +5471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>4</v>
       </c>
@@ -5504,7 +5522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>22</v>
       </c>
@@ -5555,7 +5573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>22</v>
       </c>
@@ -5606,7 +5624,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>4</v>
       </c>
@@ -5657,7 +5675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>4</v>
       </c>
@@ -5708,7 +5726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>22</v>
       </c>
@@ -5759,7 +5777,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>4</v>
       </c>
@@ -5810,7 +5828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>22</v>
       </c>
@@ -5861,7 +5879,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>22</v>
       </c>
@@ -5912,7 +5930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>24</v>
       </c>
@@ -5921,7 +5939,7 @@
         <v>p</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>32</v>
@@ -5966,7 +5984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>22</v>
       </c>
@@ -6017,7 +6035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>22</v>
       </c>
@@ -6068,7 +6086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>24</v>
       </c>
@@ -6077,7 +6095,7 @@
         <v>p</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>33</v>
@@ -6122,7 +6140,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>22</v>
       </c>
@@ -6173,7 +6191,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>22</v>
       </c>
@@ -6224,7 +6242,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>24</v>
       </c>
@@ -6297,8 +6315,8 @@
   </sheetPr>
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C47" activeCellId="0" sqref="C47"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -7036,66 +7054,66 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="0" t="str">
+      <c r="B13" s="2" t="str">
         <f aca="false">VLOOKUP(LEFT(A13, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="0" t="s">
+      <c r="C13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="3" t="n">
         <v>89</v>
       </c>
-      <c r="F13" s="1" t="n">
+      <c r="F13" s="3" t="n">
         <v>702</v>
       </c>
-      <c r="G13" s="1" t="n">
+      <c r="G13" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="H13" s="1" t="n">
+      <c r="H13" s="3" t="n">
         <v>282</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O13" s="1" t="n">
+      <c r="I13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="P13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="T13" s="1" t="n">
+      <c r="P13" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="T13" s="3" t="n">
         <v>2</v>
       </c>
     </row>
@@ -7459,66 +7477,66 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="0" t="str">
+      <c r="B20" s="2" t="str">
         <f aca="false">VLOOKUP(LEFT(A20, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
-      <c r="C20" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="0" t="s">
+      <c r="C20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="F20" s="1" t="n">
+      <c r="E20" s="3" t="n">
+        <v>121</v>
+      </c>
+      <c r="F20" s="3" t="n">
         <v>3293</v>
       </c>
-      <c r="G20" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H20" s="1" t="n">
+      <c r="G20" s="3" t="n">
+        <v>117</v>
+      </c>
+      <c r="H20" s="3" t="n">
         <v>3302</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O20" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="P20" s="1" t="n">
+      <c r="I20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O20" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P20" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="Q20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="T20" s="1" t="n">
+      <c r="Q20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="T20" s="3" t="n">
         <v>2</v>
       </c>
     </row>
@@ -9713,8 +9731,8 @@
   </sheetPr>
   <dimension ref="A1:Q72"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C68" activeCellId="0" sqref="C68"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C53" activeCellId="0" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -10443,57 +10461,57 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="0" t="str">
+      <c r="B15" s="2" t="str">
         <f aca="false">VLOOKUP(LEFT(A15, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="0" t="s">
+      <c r="C15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="F15" s="1" t="n">
+      <c r="F15" s="3" t="n">
         <v>702</v>
       </c>
-      <c r="G15" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H15" s="1" t="n">
+      <c r="G15" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3" t="n">
         <v>282</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M15" s="1" t="n">
+      <c r="I15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M15" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="N15" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q15" s="1" t="n">
+      <c r="N15" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q15" s="3" t="n">
         <v>2</v>
       </c>
     </row>
@@ -10599,57 +10617,57 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="0" t="str">
+      <c r="B18" s="2" t="str">
         <f aca="false">VLOOKUP(LEFT(A18, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="0" t="s">
+      <c r="C18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="1" t="n">
+      <c r="E18" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="F18" s="1" t="n">
+      <c r="F18" s="3" t="n">
         <v>3301</v>
       </c>
-      <c r="G18" s="1" t="n">
+      <c r="G18" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="H18" s="1" t="n">
+      <c r="H18" s="3" t="n">
         <v>3304</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M18" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N18" s="1" t="n">
+      <c r="I18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M18" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N18" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="O18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q18" s="1" t="n">
+      <c r="O18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q18" s="3" t="n">
         <v>2</v>
       </c>
     </row>
@@ -11013,57 +11031,57 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="26" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="0" t="str">
+      <c r="B26" s="2" t="str">
         <f aca="false">VLOOKUP(LEFT(A26, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="0" t="s">
+      <c r="C26" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="1" t="n">
+      <c r="D26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="F26" s="1" t="n">
+      <c r="F26" s="3" t="n">
         <v>223</v>
       </c>
-      <c r="G26" s="1" t="n">
+      <c r="G26" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="H26" s="1" t="n">
+      <c r="H26" s="3" t="n">
         <v>224</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M26" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N26" s="1" t="n">
+      <c r="I26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M26" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N26" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="O26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q26" s="1" t="n">
+      <c r="O26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q26" s="3" t="n">
         <v>2</v>
       </c>
     </row>
@@ -11118,57 +11136,57 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+    <row r="28" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="0" t="str">
+      <c r="B28" s="2" t="str">
         <f aca="false">VLOOKUP(LEFT(A28, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
-      <c r="C28" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D28" s="0" t="s">
+      <c r="C28" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E28" s="1" t="n">
+      <c r="E28" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="F28" s="1" t="n">
+      <c r="F28" s="3" t="n">
         <v>3293</v>
       </c>
-      <c r="G28" s="1" t="n">
+      <c r="G28" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="H28" s="1" t="n">
+      <c r="H28" s="3" t="n">
         <v>3302</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M28" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N28" s="1" t="n">
+      <c r="I28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M28" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N28" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="O28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q28" s="1" t="n">
+      <c r="O28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q28" s="3" t="n">
         <v>2</v>
       </c>
     </row>
@@ -12357,7 +12375,7 @@
         <v>p</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>32</v>
@@ -13447,31 +13465,31 @@
   </sheetPr>
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C48" activeCellId="0" sqref="C48"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="26.3740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="9.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="6.75555555555556"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="19.1296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="26.3740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="9.5"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="6.75555555555556"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="19.1296296296296"/>
     <col collapsed="false" hidden="false" max="15" min="5" style="1" width="10.8777777777778"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -13515,14 +13533,14 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="str">
+      <c r="B2" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A2, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>m</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="0"/>
@@ -13567,14 +13585,14 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="str">
+      <c r="B3" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A3, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>m</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="0"/>
@@ -13619,14 +13637,14 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="2" t="str">
+      <c r="B4" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A4, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>s</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="0"/>
@@ -13671,14 +13689,14 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="str">
+      <c r="B5" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A5, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>m</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="0"/>
@@ -13723,14 +13741,14 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="2" t="str">
+      <c r="B6" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A6, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="0"/>
@@ -13775,14 +13793,14 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2" t="str">
+      <c r="B7" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A7, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>m</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="0"/>
@@ -13827,14 +13845,14 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2" t="str">
+      <c r="B8" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A8, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>m</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="0"/>
@@ -13879,14 +13897,14 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="2" t="str">
+      <c r="B9" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A9, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>s</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="0"/>
@@ -13931,14 +13949,14 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="2" t="str">
+      <c r="B10" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A10, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="0"/>
@@ -13982,69 +14000,69 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+    <row r="11" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="2" t="str">
+      <c r="B11" s="5" t="str">
         <f aca="false">VLOOKUP(LEFT(A11, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="C11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="F11" s="1" t="n">
+      <c r="F11" s="3" t="n">
         <v>702</v>
       </c>
-      <c r="G11" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H11" s="1" t="n">
+      <c r="G11" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3" t="n">
         <v>282</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M11" s="1" t="n">
+      <c r="I11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="N11" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q11" s="1" t="n">
+      <c r="N11" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q11" s="3" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="2" t="str">
+      <c r="B12" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A12, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>s</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="0"/>
@@ -14088,69 +14106,69 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+    <row r="13" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="2" t="str">
+      <c r="B13" s="5" t="str">
         <f aca="false">VLOOKUP(LEFT(A13, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="C13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="F13" s="1" t="n">
+      <c r="E13" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="F13" s="3" t="n">
         <v>3301</v>
       </c>
-      <c r="G13" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="H13" s="1" t="n">
+      <c r="G13" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="H13" s="3" t="n">
         <v>3304</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N13" s="1" t="n">
+      <c r="I13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="O13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q13" s="1" t="n">
+      <c r="O13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q13" s="3" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="2" t="str">
+      <c r="B14" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A14, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>s</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D14" s="0"/>
@@ -14195,14 +14213,14 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="2" t="str">
+      <c r="B15" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A15, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>s</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="0"/>
@@ -14247,14 +14265,14 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="2" t="str">
+      <c r="B16" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A16, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>s</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="0"/>
@@ -14299,14 +14317,14 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="2" t="str">
+      <c r="B17" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A17, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>s</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D17" s="0"/>
@@ -14351,14 +14369,14 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="2" t="str">
+      <c r="B18" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A18, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>s</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D18" s="0"/>
@@ -14402,123 +14420,123 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+    <row r="19" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="2" t="str">
+      <c r="B19" s="5" t="str">
         <f aca="false">VLOOKUP(LEFT(A19, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="C19" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="1" t="n">
+      <c r="D19" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="F19" s="1" t="n">
+      <c r="F19" s="3" t="n">
         <v>223</v>
       </c>
-      <c r="G19" s="1" t="n">
+      <c r="G19" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="H19" s="1" t="n">
+      <c r="H19" s="3" t="n">
         <v>224</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M19" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N19" s="1" t="n">
+      <c r="I19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M19" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N19" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="O19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q19" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
+      <c r="O19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q19" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="2" t="str">
+      <c r="B20" s="5" t="str">
         <f aca="false">VLOOKUP(LEFT(A20, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="2" t="s">
+      <c r="C20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F20" s="1" t="n">
+      <c r="E20" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3" t="n">
         <v>3293</v>
       </c>
-      <c r="G20" s="1" t="n">
+      <c r="G20" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="H20" s="1" t="n">
+      <c r="H20" s="3" t="n">
         <v>3302</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M20" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N20" s="1" t="n">
+      <c r="I20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M20" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N20" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="O20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q20" s="1" t="n">
+      <c r="O20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q20" s="3" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="2" t="str">
+      <c r="B21" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A21, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>s</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D21" s="0"/>
@@ -14563,14 +14581,14 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="2" t="str">
+      <c r="B22" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A22, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>m</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="0"/>
@@ -14615,14 +14633,14 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="2" t="str">
+      <c r="B23" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A23, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>m</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="0"/>
@@ -14667,14 +14685,14 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="2" t="str">
+      <c r="B24" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A24, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>s</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D24" s="0"/>
@@ -14719,14 +14737,14 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="2" t="str">
+      <c r="B25" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A25, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>s</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="0"/>
@@ -14771,14 +14789,14 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="2" t="str">
+      <c r="B26" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A26, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>s</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D26" s="0"/>
@@ -14823,14 +14841,14 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="2" t="str">
+      <c r="B27" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A27, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>s</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D27" s="0"/>
@@ -14875,17 +14893,17 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="2" t="str">
+      <c r="B28" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A28, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="C28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E28" s="1" t="n">
@@ -14929,14 +14947,14 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="2" t="str">
+      <c r="B29" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A29, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>s</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D29" s="0"/>
@@ -14981,14 +14999,14 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="2" t="str">
+      <c r="B30" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A30, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>s</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="0"/>
@@ -15033,14 +15051,14 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="2" t="str">
+      <c r="B31" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A31, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>s</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D31" s="0"/>
@@ -15085,17 +15103,17 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="2" t="str">
+      <c r="B32" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A32, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" s="2" t="s">
+      <c r="C32" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E32" s="1" t="n">
@@ -15139,14 +15157,14 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="2" t="str">
+      <c r="B33" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A33, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>s</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D33" s="0"/>
@@ -15191,14 +15209,14 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="2" t="str">
+      <c r="B34" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A34, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D34" s="0"/>
@@ -15243,14 +15261,14 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="2" t="str">
+      <c r="B35" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A35, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>m</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D35" s="0"/>
@@ -15295,14 +15313,14 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="2" t="str">
+      <c r="B36" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A36, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>s</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D36" s="0"/>
@@ -15347,14 +15365,14 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="2" t="str">
+      <c r="B37" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A37, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>s</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D37" s="0"/>
@@ -15399,14 +15417,14 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B38" s="2" t="str">
+      <c r="B38" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A38, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>s</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D38" s="0"/>
@@ -15451,17 +15469,17 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="2" t="str">
+      <c r="B39" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A39, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D39" s="2" t="s">
+      <c r="C39" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>32</v>
       </c>
       <c r="E39" s="1" t="n">
@@ -15505,14 +15523,14 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="2" t="str">
+      <c r="B40" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A40, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>s</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D40" s="0"/>
@@ -15557,17 +15575,17 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="2" t="str">
+      <c r="B41" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A41, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D41" s="2" t="s">
+      <c r="C41" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E41" s="1" t="n">
@@ -15611,14 +15629,14 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B42" s="2" t="str">
+      <c r="B42" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A42, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>s</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D42" s="0"/>
@@ -15663,17 +15681,17 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="2" t="str">
+      <c r="B43" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A43, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D43" s="2" t="s">
+      <c r="C43" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>54</v>
       </c>
       <c r="E43" s="1" t="n">
@@ -15717,14 +15735,14 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="2" t="str">
+      <c r="B44" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A44, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>m</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D44" s="0"/>
@@ -15769,14 +15787,14 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="2" t="str">
+      <c r="B45" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A45, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>m</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D45" s="0"/>
@@ -15821,14 +15839,14 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B46" s="2" t="str">
+      <c r="B46" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A46, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>s</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D46" s="0"/>
@@ -15873,14 +15891,14 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="2" t="str">
+      <c r="B47" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A47, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>m</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D47" s="0"/>
@@ -15925,14 +15943,14 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="2" t="str">
+      <c r="B48" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A48, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>m</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D48" s="0"/>
@@ -15977,17 +15995,17 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B49" s="2" t="str">
+      <c r="B49" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A49, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>p</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D49" s="2" t="s">
+      <c r="C49" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D49" s="4" t="s">
         <v>49</v>
       </c>
       <c r="E49" s="1" t="n">
@@ -16031,14 +16049,14 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B50" s="2" t="str">
+      <c r="B50" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A50, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>m</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E50" s="1" t="n">
@@ -16082,14 +16100,14 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B51" s="2" t="str">
+      <c r="B51" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A51, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>m</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E51" s="1" t="n">
@@ -16133,14 +16151,14 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B52" s="2" t="str">
+      <c r="B52" s="4" t="str">
         <f aca="false">VLOOKUP(LEFT(A52, 5)&amp;"*", vals!$A$1:$B$3, 2, 0)</f>
         <v>m</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E52" s="1" t="n">

</xml_diff>